<commit_message>
updated calculator with updated result
</commit_message>
<xml_diff>
--- a/Preethi/RoboticEnterpriseFramework1Calculator/Data/Input/input.xlsx
+++ b/Preethi/RoboticEnterpriseFramework1Calculator/Data/Input/input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uipath\GitSpace\RPA-Developer-in-30-Days\vajrang\Week1Calculator_Reframework\Data\Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sridh\OneDrive\Documents\RPA-Developer-in-30-Days\Preethi\RoboticEnterpriseFramework1Calculator\Data\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD8872B9-BC25-43BC-97D1-BC1AE163CD6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBCFC940-925A-4766-972E-077CBC4B2FC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11490" yWindow="360" windowWidth="5565" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>first</t>
   </si>
@@ -43,6 +43,33 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8	
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10	
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27	
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0	
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5	
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4	
+</t>
   </si>
 </sst>
 </file>
@@ -78,8 +105,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -360,15 +390,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -378,8 +408,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -389,8 +422,11 @@
       <c r="C2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -400,8 +436,11 @@
       <c r="C3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -411,8 +450,11 @@
       <c r="C4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D4" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -422,8 +464,11 @@
       <c r="C5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D5" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -433,8 +478,11 @@
       <c r="C6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D6" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -443,6 +491,9 @@
       </c>
       <c r="C7" t="s">
         <v>5</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>